<commit_message>
Add push/pull timing to the code base. Keep getting performance metricx
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E666FC09-F02C-42B1-8A10-E2596373F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992B3BD-2D57-4551-8EEB-4AF4BA4E1B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-9610" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-34090" yWindow="-9430" windowWidth="21600" windowHeight="12640" activeTab="3" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
     <sheet name="Pubsub" sheetId="2" r:id="rId2"/>
     <sheet name="ReqReply" sheetId="3" r:id="rId3"/>
+    <sheet name="PushPull" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Pair</t>
   </si>
@@ -117,13 +118,27 @@
   <si>
     <t>Small kb/sec</t>
   </si>
+  <si>
+    <t>tcp: 10000 msgs</t>
+  </si>
+  <si>
+    <t>Pullers:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -151,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -159,6 +174,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16112,7 +16128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03558752-A656-4B2D-A4F2-0A2EF9D8FEE1}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
@@ -16357,4 +16373,70 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39964DF-471C-4FDD-B17E-1787F531762F}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update with push/pull timings.
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33657AE-ED75-4352-802C-D442240F88F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE01A3D1-EB77-4E35-94BB-4D05D7E0AE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34690" yWindow="-9120" windowWidth="34480" windowHeight="14840" activeTab="3" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-35640" yWindow="-9260" windowWidth="34480" windowHeight="14840" activeTab="3" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Pair</t>
   </si>
@@ -3532,10 +3532,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$26</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -3565,16 +3565,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$B$17:$B$26</c:f>
+              <c:f>PushPull!$B$17:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>6188</c:v>
                 </c:pt>
@@ -3604,6 +3607,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2809</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3647,10 +3653,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$26</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -3680,16 +3686,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$D$17:$D$26</c:f>
+              <c:f>PushPull!$D$17:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5236</c:v>
                 </c:pt>
@@ -3719,6 +3728,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2555</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3762,10 +3774,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$25</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -3792,16 +3804,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$F$17:$F$25</c:f>
+              <c:f>PushPull!$F$17:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5844</c:v>
                 </c:pt>
@@ -3828,6 +3846,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3493</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2332</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3871,10 +3895,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$25</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -3901,16 +3925,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$H$17:$H$25</c:f>
+              <c:f>PushPull!$H$17:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5810</c:v>
                 </c:pt>
@@ -3937,6 +3967,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2542</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4388,10 +4424,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$26</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -4421,16 +4457,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$C$17:$C$26</c:f>
+              <c:f>PushPull!$C$17:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>6188</c:v>
                 </c:pt>
@@ -4460,6 +4499,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1440000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1400000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4503,10 +4545,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$26</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -4536,16 +4578,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$E$17:$E$26</c:f>
+              <c:f>PushPull!$E$17:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5236</c:v>
                 </c:pt>
@@ -4575,6 +4620,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1310000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4618,10 +4666,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$25</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -4648,16 +4696,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$G$17:$G$25</c:f>
+              <c:f>PushPull!$G$17:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5844</c:v>
                 </c:pt>
@@ -4684,6 +4738,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>894167</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1190000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1360000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4727,10 +4787,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>PushPull!$A$17:$A$25</c:f>
+              <c:f>PushPull!$A$17:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -4757,16 +4817,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PushPull!$I$17:$I$25</c:f>
+              <c:f>PushPull!$I$17:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>5810</c:v>
                 </c:pt>
@@ -4793,6 +4859,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>940140</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1300000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1260000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5046,6 +5118,1803 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="119773632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>push/sec as a function</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of message size and nof pullers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.890266841644795E-2"/>
+          <c:y val="1.8518518518518517E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1 puller</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$B$33:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4472</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4924</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4735</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5322</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5203</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4719</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5362</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7764</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7936</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-902F-4B8A-9154-D4B1C91993F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2 pul.lers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$D$33:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7831</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7513</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8969</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8554</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10684</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10718</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10537</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-902F-4B8A-9154-D4B1C91993F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3 pullers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$F$33:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6978</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10917</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11312</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-902F-4B8A-9154-D4B1C91993F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>4 pullers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$H$33:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7576</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8628</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9634</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12092</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11416</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10526</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6013</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-902F-4B8A-9154-D4B1C91993F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="124316400"/>
+        <c:axId val="124313040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="124316400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size in bytes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="124313040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="124313040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PUshes/sec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="124316400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kb</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> pushed/sec as a function of msg size and nof pullers</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1 puller</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$C$33:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166493</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>302029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>686327</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>1990000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>4060000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>6850000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2340-416B-925D-829DA23374A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2 pullers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$E$33:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>286996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>547476</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1370000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2740000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5400000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>5920000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2340-416B-925D-829DA23374A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>3 pullers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$G$33:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124420</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55827</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>126482</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640641</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1400000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2050000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5790000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>6210000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2340-416B-925D-829DA23374A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>4 pullers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PushPull!$A$33:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PushPull!$I$33:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14174</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>122137</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>276100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>616570</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1550000</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2920000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>5390000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>6160000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2340-416B-925D-829DA23374A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1336095328"/>
+        <c:axId val="120322272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1336095328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in bytes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="120322272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120322272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KB pushed/sec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1336095328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12107,6 +13976,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -15008,6 +16957,1038 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20172,6 +23153,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>454024</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>431799</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FE6603B-2D20-F6C9-01D8-AC8853F40E92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>517525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E973BF32-D26C-DED2-FBE5-5DC3B2EACF51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -22249,10 +25302,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39964DF-471C-4FDD-B17E-1787F531762F}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="AA58" sqref="AA58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22926,11 +25979,375 @@
       <c r="E26" s="2">
         <v>1310000</v>
       </c>
+      <c r="F26">
+        <v>2332</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1190000</v>
+      </c>
+      <c r="H26">
+        <v>2542</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1300000</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>2*A26</f>
         <v>1048576</v>
+      </c>
+      <c r="B27">
+        <v>1367</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1400000</v>
+      </c>
+      <c r="D27">
+        <v>1428</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="F27">
+        <v>1325</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1360000</v>
+      </c>
+      <c r="H27">
+        <v>1235</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1260000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1024</v>
+      </c>
+      <c r="B33">
+        <v>5184</v>
+      </c>
+      <c r="C33">
+        <v>5184</v>
+      </c>
+      <c r="D33">
+        <v>7205</v>
+      </c>
+      <c r="E33">
+        <v>7205</v>
+      </c>
+      <c r="F33">
+        <v>7062</v>
+      </c>
+      <c r="G33">
+        <v>7062</v>
+      </c>
+      <c r="H33">
+        <v>7407</v>
+      </c>
+      <c r="I33">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2048</v>
+      </c>
+      <c r="B34">
+        <v>4472</v>
+      </c>
+      <c r="C34">
+        <v>8944</v>
+      </c>
+      <c r="D34">
+        <v>7831</v>
+      </c>
+      <c r="E34">
+        <v>15662</v>
+      </c>
+      <c r="F34">
+        <v>7209</v>
+      </c>
+      <c r="G34">
+        <v>124420</v>
+      </c>
+      <c r="H34">
+        <v>7087</v>
+      </c>
+      <c r="I34">
+        <v>14174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4096</v>
+      </c>
+      <c r="B35">
+        <v>4924</v>
+      </c>
+      <c r="C35">
+        <v>19695</v>
+      </c>
+      <c r="D35">
+        <v>7402</v>
+      </c>
+      <c r="E35">
+        <v>29608</v>
+      </c>
+      <c r="F35">
+        <v>8643</v>
+      </c>
+      <c r="G35">
+        <v>69144</v>
+      </c>
+      <c r="H35">
+        <v>9268</v>
+      </c>
+      <c r="I35">
+        <v>74143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8192</v>
+      </c>
+      <c r="B36">
+        <v>4735</v>
+      </c>
+      <c r="C36">
+        <v>37879</v>
+      </c>
+      <c r="D36">
+        <v>7513</v>
+      </c>
+      <c r="E36">
+        <v>60105</v>
+      </c>
+      <c r="F36">
+        <v>6978</v>
+      </c>
+      <c r="G36">
+        <v>55827</v>
+      </c>
+      <c r="H36">
+        <v>7576</v>
+      </c>
+      <c r="I36">
+        <v>60606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16384</v>
+      </c>
+      <c r="B37">
+        <v>5322</v>
+      </c>
+      <c r="C37">
+        <v>85152</v>
+      </c>
+      <c r="D37">
+        <v>7794</v>
+      </c>
+      <c r="E37">
+        <v>124708</v>
+      </c>
+      <c r="F37">
+        <v>7905</v>
+      </c>
+      <c r="G37">
+        <v>126482</v>
+      </c>
+      <c r="H37">
+        <v>4634</v>
+      </c>
+      <c r="I37">
+        <v>122137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32768</v>
+      </c>
+      <c r="B38">
+        <v>5203</v>
+      </c>
+      <c r="C38">
+        <v>166493</v>
+      </c>
+      <c r="D38">
+        <v>8969</v>
+      </c>
+      <c r="E38">
+        <v>286996</v>
+      </c>
+      <c r="F38">
+        <v>9216</v>
+      </c>
+      <c r="G38">
+        <v>294931</v>
+      </c>
+      <c r="H38">
+        <v>8628</v>
+      </c>
+      <c r="I38">
+        <v>276100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>65536</v>
+      </c>
+      <c r="B39">
+        <v>4719</v>
+      </c>
+      <c r="C39">
+        <v>302029</v>
+      </c>
+      <c r="D39">
+        <v>8554</v>
+      </c>
+      <c r="E39">
+        <v>547476</v>
+      </c>
+      <c r="F39">
+        <v>10010</v>
+      </c>
+      <c r="G39">
+        <v>640641</v>
+      </c>
+      <c r="H39">
+        <v>9634</v>
+      </c>
+      <c r="I39">
+        <v>616570</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>2*A39</f>
+        <v>131072</v>
+      </c>
+      <c r="B40">
+        <v>5362</v>
+      </c>
+      <c r="C40">
+        <v>686327</v>
+      </c>
+      <c r="D40">
+        <v>10684</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1370000</v>
+      </c>
+      <c r="F40">
+        <v>10917</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1400000</v>
+      </c>
+      <c r="H40">
+        <v>12092</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1550000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>A40*2</f>
+        <v>262144</v>
+      </c>
+      <c r="B41">
+        <v>7764</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1990000</v>
+      </c>
+      <c r="D41">
+        <v>10718</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2740000</v>
+      </c>
+      <c r="F41">
+        <v>8000</v>
+      </c>
+      <c r="G41" s="2">
+        <v>2050000</v>
+      </c>
+      <c r="H41">
+        <v>11416</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2920000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>A41*2</f>
+        <v>524288</v>
+      </c>
+      <c r="B42">
+        <v>7936</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4060000</v>
+      </c>
+      <c r="D42">
+        <v>10537</v>
+      </c>
+      <c r="E42" s="2">
+        <v>5400000</v>
+      </c>
+      <c r="F42">
+        <v>11312</v>
+      </c>
+      <c r="G42" s="2">
+        <v>5790000</v>
+      </c>
+      <c r="H42">
+        <v>10526</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5390000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>2*A42</f>
+        <v>1048576</v>
+      </c>
+      <c r="B43">
+        <v>6693</v>
+      </c>
+      <c r="C43" s="2">
+        <v>6850000</v>
+      </c>
+      <c r="D43">
+        <v>5780</v>
+      </c>
+      <c r="E43" s="2">
+        <v>5920000</v>
+      </c>
+      <c r="F43">
+        <v>6064</v>
+      </c>
+      <c r="G43" s="2">
+        <v>6210000</v>
+      </c>
+      <c r="H43">
+        <v>6013</v>
+      </c>
+      <c r="I43" s="2">
+        <v>6160000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*   Added survey.cpp - timing suvey/responder. *   Added to build. *   Make a new spreadsheet page on which to capture timings.
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF95F50-2E27-4717-82D3-4EF5F86B4C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6280BC78-D1C0-486F-AF6C-599A29FFF095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35640" yWindow="-9260" windowWidth="34480" windowHeight="14840" activeTab="3" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-37040" yWindow="-9500" windowWidth="34490" windowHeight="14840" activeTab="4" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
     <sheet name="Pubsub" sheetId="2" r:id="rId2"/>
     <sheet name="ReqReply" sheetId="3" r:id="rId3"/>
     <sheet name="PushPull" sheetId="4" r:id="rId4"/>
+    <sheet name="SurveyRespnod" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Pair</t>
   </si>
@@ -127,6 +128,39 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>tcp:</t>
+  </si>
+  <si>
+    <t>10000 survyeys</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>big surveys/sec</t>
+  </si>
+  <si>
+    <t>big KBs</t>
+  </si>
+  <si>
+    <t>small surveys/sec</t>
+  </si>
+  <si>
+    <t>small KBs</t>
+  </si>
+  <si>
+    <t>1 responder</t>
+  </si>
+  <si>
+    <t>2 responders</t>
+  </si>
+  <si>
+    <t>3 responders</t>
+  </si>
+  <si>
+    <t>4responders</t>
+  </si>
 </sst>
 </file>
 
@@ -173,11 +207,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24006,13 +24040,13 @@
       <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -24030,13 +24064,13 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -24066,11 +24100,11 @@
       <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -25304,7 +25338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39964DF-471C-4FDD-B17E-1787F531762F}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+    <sheetView topLeftCell="B28" workbookViewId="0">
       <selection activeCell="AA58" sqref="AA58"/>
     </sheetView>
   </sheetViews>
@@ -25319,7 +25353,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2">
@@ -26354,4 +26388,188 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3168BB-833A-4FB7-A9ED-74D6E2A3DEE5}">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1024</v>
+      </c>
+      <c r="B4">
+        <v>1935</v>
+      </c>
+      <c r="C4">
+        <v>1935</v>
+      </c>
+      <c r="D4">
+        <v>2284</v>
+      </c>
+      <c r="E4">
+        <v>2284</v>
+      </c>
+      <c r="F4">
+        <v>1250</v>
+      </c>
+      <c r="G4">
+        <v>1250</v>
+      </c>
+      <c r="H4">
+        <v>1371</v>
+      </c>
+      <c r="I4">
+        <v>2742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8*2</f>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9*2</f>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10*2</f>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11*2</f>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12*2</f>
+        <v>1048576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* Increase survey timeout to 8seconds so big resopnses can be read. * Collect more data on survey/response.
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6280BC78-D1C0-486F-AF6C-599A29FFF095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B710E875-F176-4B76-96B6-269DBD041E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37040" yWindow="-9500" windowWidth="34490" windowHeight="14840" activeTab="4" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-38200" yWindow="-9440" windowWidth="34490" windowHeight="14840" activeTab="4" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="51">
   <si>
     <t>Pair</t>
   </si>
@@ -160,6 +160,39 @@
   </si>
   <si>
     <t>4responders</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>failure</t>
+  </si>
+  <si>
+    <t>FAILURE</t>
+  </si>
+  <si>
+    <t>ipc:</t>
+  </si>
+  <si>
+    <t>1 repond</t>
+  </si>
+  <si>
+    <t>2 repond</t>
+  </si>
+  <si>
+    <t>4 respond</t>
+  </si>
+  <si>
+    <t>3 respond</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
@@ -26392,10 +26425,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3168BB-833A-4FB7-A9ED-74D6E2A3DEE5}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:S3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26407,6 +26440,12 @@
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -26472,22 +26511,19 @@
         <v>35</v>
       </c>
       <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" t="s">
-        <v>34</v>
-      </c>
       <c r="S3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -26495,78 +26531,1248 @@
         <v>1024</v>
       </c>
       <c r="B4">
-        <v>1935</v>
+        <v>2614</v>
       </c>
       <c r="C4">
-        <v>1935</v>
+        <v>2164</v>
       </c>
       <c r="D4">
-        <v>2284</v>
+        <v>2472</v>
       </c>
       <c r="E4">
-        <v>2284</v>
+        <v>2472</v>
       </c>
       <c r="F4">
-        <v>1250</v>
+        <v>1422</v>
       </c>
       <c r="G4">
-        <v>1250</v>
+        <v>1422</v>
       </c>
       <c r="H4">
-        <v>1371</v>
+        <v>1432</v>
       </c>
       <c r="I4">
-        <v>2742</v>
+        <v>2863</v>
+      </c>
+      <c r="J4">
+        <v>992</v>
+      </c>
+      <c r="K4">
+        <v>992</v>
+      </c>
+      <c r="L4">
+        <v>809</v>
+      </c>
+      <c r="M4">
+        <v>2427</v>
+      </c>
+      <c r="N4">
+        <v>682</v>
+      </c>
+      <c r="O4">
+        <v>682</v>
+      </c>
+      <c r="P4">
+        <v>749</v>
+      </c>
+      <c r="Q4">
+        <v>2998</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2048</v>
       </c>
+      <c r="B5">
+        <v>2419</v>
+      </c>
+      <c r="C5">
+        <v>4838</v>
+      </c>
+      <c r="D5">
+        <v>2082</v>
+      </c>
+      <c r="E5">
+        <v>4163</v>
+      </c>
+      <c r="F5">
+        <v>1380</v>
+      </c>
+      <c r="G5">
+        <v>2759</v>
+      </c>
+      <c r="H5">
+        <v>1345</v>
+      </c>
+      <c r="I5">
+        <v>5380</v>
+      </c>
+      <c r="J5">
+        <v>1001</v>
+      </c>
+      <c r="K5">
+        <v>2001</v>
+      </c>
+      <c r="L5">
+        <v>910</v>
+      </c>
+      <c r="M5">
+        <v>5462</v>
+      </c>
+      <c r="N5">
+        <v>700</v>
+      </c>
+      <c r="O5">
+        <v>1399</v>
+      </c>
+      <c r="P5">
+        <v>713</v>
+      </c>
+      <c r="Q5">
+        <v>5701</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4096</v>
       </c>
+      <c r="B6">
+        <v>2458</v>
+      </c>
+      <c r="C6">
+        <v>9830</v>
+      </c>
+      <c r="D6">
+        <v>1911</v>
+      </c>
+      <c r="E6">
+        <v>7644</v>
+      </c>
+      <c r="F6">
+        <v>1367</v>
+      </c>
+      <c r="G6">
+        <v>5467</v>
+      </c>
+      <c r="H6">
+        <v>1200</v>
+      </c>
+      <c r="I6">
+        <v>9602</v>
+      </c>
+      <c r="J6">
+        <v>943</v>
+      </c>
+      <c r="K6">
+        <v>3771</v>
+      </c>
+      <c r="L6">
+        <v>878</v>
+      </c>
+      <c r="M6">
+        <v>10530</v>
+      </c>
+      <c r="N6">
+        <v>751</v>
+      </c>
+      <c r="O6">
+        <v>3003</v>
+      </c>
+      <c r="P6">
+        <v>672</v>
+      </c>
+      <c r="Q6">
+        <v>10760</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16384</v>
+        <v>8192</v>
+      </c>
+      <c r="B7">
+        <v>2602</v>
+      </c>
+      <c r="C7">
+        <v>20817</v>
+      </c>
+      <c r="D7">
+        <v>1911</v>
+      </c>
+      <c r="E7">
+        <v>15288</v>
+      </c>
+      <c r="F7">
+        <v>1263</v>
+      </c>
+      <c r="G7">
+        <v>10101</v>
+      </c>
+      <c r="H7">
+        <v>1038</v>
+      </c>
+      <c r="I7">
+        <v>16613</v>
+      </c>
+      <c r="J7">
+        <v>974</v>
+      </c>
+      <c r="K7">
+        <v>7796</v>
+      </c>
+      <c r="L7">
+        <v>899</v>
+      </c>
+      <c r="M7">
+        <v>21581</v>
+      </c>
+      <c r="N7">
+        <v>681</v>
+      </c>
+      <c r="O7">
+        <v>5447</v>
+      </c>
+      <c r="P7">
+        <v>724</v>
+      </c>
+      <c r="Q7">
+        <v>23187</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>32768</v>
+        <v>16384</v>
+      </c>
+      <c r="B8">
+        <v>2064</v>
+      </c>
+      <c r="C8">
+        <v>33017</v>
+      </c>
+      <c r="D8">
+        <v>1596</v>
+      </c>
+      <c r="E8">
+        <v>25543</v>
+      </c>
+      <c r="F8">
+        <v>1371</v>
+      </c>
+      <c r="G8">
+        <v>21939</v>
+      </c>
+      <c r="H8">
+        <v>1332</v>
+      </c>
+      <c r="I8">
+        <v>42633</v>
+      </c>
+      <c r="J8">
+        <v>955</v>
+      </c>
+      <c r="K8">
+        <v>15286</v>
+      </c>
+      <c r="L8">
+        <v>822</v>
+      </c>
+      <c r="M8">
+        <v>39483</v>
+      </c>
+      <c r="N8">
+        <v>697</v>
+      </c>
+      <c r="O8">
+        <v>11151</v>
+      </c>
+      <c r="P8">
+        <v>702</v>
+      </c>
+      <c r="Q8">
+        <v>44909</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>A8*2</f>
-        <v>65536</v>
+        <v>32768</v>
+      </c>
+      <c r="B9">
+        <v>2209</v>
+      </c>
+      <c r="C9">
+        <v>70703</v>
+      </c>
+      <c r="D9">
+        <v>1326</v>
+      </c>
+      <c r="E9">
+        <v>42418</v>
+      </c>
+      <c r="F9">
+        <v>1357</v>
+      </c>
+      <c r="G9">
+        <v>43437</v>
+      </c>
+      <c r="H9">
+        <v>997</v>
+      </c>
+      <c r="I9">
+        <v>63783</v>
+      </c>
+      <c r="J9">
+        <v>957</v>
+      </c>
+      <c r="K9">
+        <v>30616</v>
+      </c>
+      <c r="L9">
+        <v>775</v>
+      </c>
+      <c r="M9">
+        <v>74401</v>
+      </c>
+      <c r="N9">
+        <v>706</v>
+      </c>
+      <c r="O9">
+        <v>22578</v>
+      </c>
+      <c r="P9">
+        <v>609</v>
+      </c>
+      <c r="Q9">
+        <v>77930</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9*2</f>
-        <v>131072</v>
+        <v>65536</v>
+      </c>
+      <c r="B10">
+        <v>1649</v>
+      </c>
+      <c r="C10">
+        <v>105558</v>
+      </c>
+      <c r="D10">
+        <v>1594</v>
+      </c>
+      <c r="E10">
+        <v>10241</v>
+      </c>
+      <c r="F10">
+        <v>1434</v>
+      </c>
+      <c r="G10">
+        <v>9183</v>
+      </c>
+      <c r="H10">
+        <v>753</v>
+      </c>
+      <c r="I10">
+        <v>96415</v>
+      </c>
+      <c r="J10">
+        <v>719</v>
+      </c>
+      <c r="K10">
+        <v>45040</v>
+      </c>
+      <c r="L10">
+        <v>714</v>
+      </c>
+      <c r="M10">
+        <v>137123</v>
+      </c>
+      <c r="N10">
+        <v>601</v>
+      </c>
+      <c r="O10">
+        <v>38448</v>
+      </c>
+      <c r="P10">
+        <v>521</v>
+      </c>
+      <c r="Q10">
+        <v>13368</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*2</f>
-        <v>262144</v>
+        <v>131072</v>
+      </c>
+      <c r="B11">
+        <v>1786</v>
+      </c>
+      <c r="C11">
+        <v>228612</v>
+      </c>
+      <c r="D11">
+        <v>961</v>
+      </c>
+      <c r="E11">
+        <v>123053</v>
+      </c>
+      <c r="F11">
+        <v>1351</v>
+      </c>
+      <c r="G11">
+        <v>172973</v>
+      </c>
+      <c r="H11">
+        <v>800</v>
+      </c>
+      <c r="I11">
+        <v>204702</v>
+      </c>
+      <c r="J11">
+        <v>667</v>
+      </c>
+      <c r="K11">
+        <v>85419</v>
+      </c>
+      <c r="L11">
+        <v>624</v>
+      </c>
+      <c r="M11">
+        <v>239641</v>
+      </c>
+      <c r="N11">
+        <v>657</v>
+      </c>
+      <c r="O11">
+        <v>84050</v>
+      </c>
+      <c r="P11">
+        <v>527</v>
+      </c>
+      <c r="Q11">
+        <v>269730</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A11*2</f>
-        <v>524288</v>
+        <v>262144</v>
+      </c>
+      <c r="B12">
+        <v>1761</v>
+      </c>
+      <c r="C12">
+        <v>450942</v>
+      </c>
+      <c r="D12">
+        <v>764</v>
+      </c>
+      <c r="E12">
+        <v>195689</v>
+      </c>
+      <c r="F12">
+        <v>1236</v>
+      </c>
+      <c r="G12">
+        <v>316479</v>
+      </c>
+      <c r="H12">
+        <v>755</v>
+      </c>
+      <c r="I12">
+        <v>386678</v>
+      </c>
+      <c r="J12">
+        <v>887</v>
+      </c>
+      <c r="K12">
+        <v>226991</v>
+      </c>
+      <c r="L12">
+        <v>338</v>
+      </c>
+      <c r="M12">
+        <v>259424</v>
+      </c>
+      <c r="N12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>A12*2</f>
+        <v>524288</v>
+      </c>
+      <c r="B13">
+        <v>1292</v>
+      </c>
+      <c r="C13">
+        <v>661328</v>
+      </c>
+      <c r="D13">
+        <v>556</v>
+      </c>
+      <c r="E13">
+        <v>284603</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" t="s">
+        <v>43</v>
+      </c>
+      <c r="P13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>A13*2</f>
         <v>1048576</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s">
+        <v>47</v>
+      </c>
+      <c r="K29" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" t="s">
+        <v>33</v>
+      </c>
+      <c r="P30" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>35</v>
+      </c>
+      <c r="S30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1024</v>
+      </c>
+      <c r="B31">
+        <v>2223.6999999999998</v>
+      </c>
+      <c r="C31">
+        <v>2223.6999999999998</v>
+      </c>
+      <c r="D31">
+        <v>1840</v>
+      </c>
+      <c r="E31">
+        <v>1840</v>
+      </c>
+      <c r="F31">
+        <v>1441</v>
+      </c>
+      <c r="G31">
+        <v>1441</v>
+      </c>
+      <c r="H31">
+        <v>1223</v>
+      </c>
+      <c r="I31">
+        <v>2445</v>
+      </c>
+      <c r="J31">
+        <v>1012</v>
+      </c>
+      <c r="K31">
+        <v>1022</v>
+      </c>
+      <c r="L31">
+        <v>1027</v>
+      </c>
+      <c r="M31">
+        <v>3082</v>
+      </c>
+      <c r="N31">
+        <v>713</v>
+      </c>
+      <c r="O31">
+        <v>713</v>
+      </c>
+      <c r="P31">
+        <v>769</v>
+      </c>
+      <c r="Q31">
+        <v>2717</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2048</v>
+      </c>
+      <c r="B32">
+        <v>2358</v>
+      </c>
+      <c r="C32">
+        <v>4716</v>
+      </c>
+      <c r="D32">
+        <v>2085</v>
+      </c>
+      <c r="E32">
+        <v>4169</v>
+      </c>
+      <c r="F32">
+        <v>1475</v>
+      </c>
+      <c r="G32">
+        <v>2949</v>
+      </c>
+      <c r="H32">
+        <v>1463</v>
+      </c>
+      <c r="I32">
+        <v>5852</v>
+      </c>
+      <c r="J32">
+        <v>1023</v>
+      </c>
+      <c r="K32">
+        <v>2046</v>
+      </c>
+      <c r="L32">
+        <v>911</v>
+      </c>
+      <c r="M32">
+        <v>5464</v>
+      </c>
+      <c r="N32">
+        <v>724</v>
+      </c>
+      <c r="O32">
+        <v>1448</v>
+      </c>
+      <c r="P32">
+        <v>736</v>
+      </c>
+      <c r="Q32">
+        <v>5336</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4096</v>
+      </c>
+      <c r="B33">
+        <v>2096</v>
+      </c>
+      <c r="C33">
+        <v>8386</v>
+      </c>
+      <c r="D33">
+        <v>1949</v>
+      </c>
+      <c r="E33">
+        <v>7796</v>
+      </c>
+      <c r="F33">
+        <v>1352</v>
+      </c>
+      <c r="G33">
+        <v>5406</v>
+      </c>
+      <c r="H33">
+        <v>1436</v>
+      </c>
+      <c r="I33">
+        <v>11489</v>
+      </c>
+      <c r="J33">
+        <v>987</v>
+      </c>
+      <c r="K33">
+        <v>3947</v>
+      </c>
+      <c r="L33">
+        <v>799</v>
+      </c>
+      <c r="M33">
+        <v>9594</v>
+      </c>
+      <c r="N33">
+        <v>736</v>
+      </c>
+      <c r="O33">
+        <v>2944</v>
+      </c>
+      <c r="P33">
+        <v>744</v>
+      </c>
+      <c r="Q33">
+        <v>11906</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8192</v>
+      </c>
+      <c r="B34">
+        <v>2039</v>
+      </c>
+      <c r="C34">
+        <v>16310</v>
+      </c>
+      <c r="D34">
+        <v>1767</v>
+      </c>
+      <c r="E34">
+        <v>14134</v>
+      </c>
+      <c r="F34">
+        <v>1423</v>
+      </c>
+      <c r="G34">
+        <v>11386</v>
+      </c>
+      <c r="H34">
+        <v>1425</v>
+      </c>
+      <c r="I34">
+        <v>22805</v>
+      </c>
+      <c r="J34">
+        <v>979</v>
+      </c>
+      <c r="K34">
+        <v>7832</v>
+      </c>
+      <c r="L34">
+        <v>657</v>
+      </c>
+      <c r="M34">
+        <v>1551</v>
+      </c>
+      <c r="N34">
+        <v>694</v>
+      </c>
+      <c r="O34">
+        <v>5554</v>
+      </c>
+      <c r="P34">
+        <v>688</v>
+      </c>
+      <c r="Q34">
+        <v>22007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>16384</v>
+      </c>
+      <c r="B35">
+        <v>2195</v>
+      </c>
+      <c r="C35">
+        <v>35126</v>
+      </c>
+      <c r="D35">
+        <v>1945</v>
+      </c>
+      <c r="E35">
+        <v>31122</v>
+      </c>
+      <c r="F35">
+        <v>1462</v>
+      </c>
+      <c r="G35">
+        <v>23392</v>
+      </c>
+      <c r="H35">
+        <v>1413</v>
+      </c>
+      <c r="I35">
+        <v>45230</v>
+      </c>
+      <c r="J35">
+        <v>869</v>
+      </c>
+      <c r="K35">
+        <v>13909</v>
+      </c>
+      <c r="L35">
+        <v>801</v>
+      </c>
+      <c r="M35">
+        <v>38465</v>
+      </c>
+      <c r="N35">
+        <v>759</v>
+      </c>
+      <c r="O35">
+        <v>12143</v>
+      </c>
+      <c r="P35">
+        <v>713</v>
+      </c>
+      <c r="Q35">
+        <v>45633</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32768</v>
+      </c>
+      <c r="B36">
+        <v>2400</v>
+      </c>
+      <c r="C36">
+        <v>76794</v>
+      </c>
+      <c r="D36">
+        <v>1612</v>
+      </c>
+      <c r="E36">
+        <v>51596</v>
+      </c>
+      <c r="F36">
+        <v>1380</v>
+      </c>
+      <c r="G36">
+        <v>44174</v>
+      </c>
+      <c r="H36">
+        <v>1350</v>
+      </c>
+      <c r="I36">
+        <v>86416</v>
+      </c>
+      <c r="J36">
+        <v>972</v>
+      </c>
+      <c r="K36">
+        <v>31122</v>
+      </c>
+      <c r="L36">
+        <v>899</v>
+      </c>
+      <c r="M36">
+        <v>86269</v>
+      </c>
+      <c r="N36">
+        <v>735</v>
+      </c>
+      <c r="O36">
+        <v>23521</v>
+      </c>
+      <c r="P36">
+        <v>632</v>
+      </c>
+      <c r="Q36">
+        <v>80931</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>A36*2</f>
+        <v>65536</v>
+      </c>
+      <c r="B37">
+        <v>2172</v>
+      </c>
+      <c r="C37">
+        <v>138979</v>
+      </c>
+      <c r="D37">
+        <v>1733</v>
+      </c>
+      <c r="E37">
+        <v>110899</v>
+      </c>
+      <c r="F37">
+        <v>1436</v>
+      </c>
+      <c r="G37">
+        <v>91901</v>
+      </c>
+      <c r="H37">
+        <v>1313</v>
+      </c>
+      <c r="I37">
+        <v>168023</v>
+      </c>
+      <c r="J37">
+        <v>964</v>
+      </c>
+      <c r="K37">
+        <v>61675</v>
+      </c>
+      <c r="L37">
+        <v>816</v>
+      </c>
+      <c r="M37">
+        <v>156581</v>
+      </c>
+      <c r="N37">
+        <v>676</v>
+      </c>
+      <c r="O37">
+        <v>43284</v>
+      </c>
+      <c r="P37">
+        <v>639</v>
+      </c>
+      <c r="Q37">
+        <v>163526</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>A37*2</f>
+        <v>131072</v>
+      </c>
+      <c r="B38">
+        <v>2012</v>
+      </c>
+      <c r="C38">
+        <v>257442</v>
+      </c>
+      <c r="D38">
+        <v>1076</v>
+      </c>
+      <c r="E38">
+        <v>137708</v>
+      </c>
+      <c r="F38">
+        <v>1323</v>
+      </c>
+      <c r="G38">
+        <v>169335</v>
+      </c>
+      <c r="H38">
+        <v>994</v>
+      </c>
+      <c r="I38">
+        <v>254574</v>
+      </c>
+      <c r="J38">
+        <v>812</v>
+      </c>
+      <c r="K38">
+        <v>103905</v>
+      </c>
+      <c r="L38">
+        <v>765</v>
+      </c>
+      <c r="M38">
+        <v>259092</v>
+      </c>
+      <c r="N38">
+        <v>648</v>
+      </c>
+      <c r="O38">
+        <v>82907</v>
+      </c>
+      <c r="P38">
+        <v>538</v>
+      </c>
+      <c r="Q38">
+        <v>275639</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>A38*2</f>
+        <v>262144</v>
+      </c>
+      <c r="B39">
+        <v>1598</v>
+      </c>
+      <c r="C39">
+        <v>409142</v>
+      </c>
+      <c r="D39">
+        <v>847</v>
+      </c>
+      <c r="E39">
+        <v>216747</v>
+      </c>
+      <c r="F39">
+        <v>1072</v>
+      </c>
+      <c r="G39">
+        <v>27443</v>
+      </c>
+      <c r="H39">
+        <v>797</v>
+      </c>
+      <c r="I39">
+        <v>407936</v>
+      </c>
+      <c r="J39">
+        <v>663</v>
+      </c>
+      <c r="K39">
+        <v>169750</v>
+      </c>
+      <c r="L39">
+        <v>303</v>
+      </c>
+      <c r="M39">
+        <v>232911</v>
+      </c>
+      <c r="N39" t="s">
+        <v>50</v>
+      </c>
+      <c r="O39" t="s">
+        <v>50</v>
+      </c>
+      <c r="P39" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>A39*2</f>
+        <v>524288</v>
+      </c>
+      <c r="B40">
+        <v>1147</v>
+      </c>
+      <c r="C40">
+        <v>587425</v>
+      </c>
+      <c r="D40">
+        <v>545</v>
+      </c>
+      <c r="E40">
+        <v>279278</v>
+      </c>
+      <c r="F40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40" t="s">
+        <v>50</v>
+      </c>
+      <c r="J40" t="s">
+        <v>50</v>
+      </c>
+      <c r="K40" t="s">
+        <v>50</v>
+      </c>
+      <c r="L40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M40" t="s">
+        <v>50</v>
+      </c>
+      <c r="N40" t="s">
+        <v>50</v>
+      </c>
+      <c r="O40" t="s">
+        <v>50</v>
+      </c>
+      <c r="P40" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>A40*2</f>
+        <v>1048576</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" t="s">
+        <v>42</v>
+      </c>
+      <c r="L41" t="s">
+        <v>42</v>
+      </c>
+      <c r="M41" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" t="s">
+        <v>42</v>
+      </c>
+      <c r="O41" t="s">
+        <v>42</v>
+      </c>
+      <c r="P41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*  Rewrite the bus measurements to try to get good shutdown and completion...still some don't. *  Update the Makefile to turn off optimization explicitly. *  Get data for bus performance.
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32661729-96E2-42D7-AABB-55BF458A1C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8949602-0745-4D64-BF1D-C587AC8BAC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38600" yWindow="-9420" windowWidth="28500" windowHeight="20660" activeTab="5" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-28770" yWindow="1830" windowWidth="28890" windowHeight="12645" activeTab="6" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="ReqReply" sheetId="3" r:id="rId3"/>
     <sheet name="PushPull" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="SurveyRespnod" sheetId="5" r:id="rId6"/>
+    <sheet name="SurveyRespond" sheetId="5" r:id="rId6"/>
+    <sheet name="Bus" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="58">
   <si>
     <t>Pair</t>
   </si>
@@ -197,6 +198,24 @@
   </si>
   <si>
     <t>2 respond</t>
+  </si>
+  <si>
+    <t>10000 full sized msgs</t>
+  </si>
+  <si>
+    <t>2000 1 byte flush msgs</t>
+  </si>
+  <si>
+    <t>KB/sec</t>
+  </si>
+  <si>
+    <t>Bus Size</t>
+  </si>
+  <si>
+    <t>Note: timings are only of full sized messages.</t>
+  </si>
+  <si>
+    <t>(at least)</t>
   </si>
 </sst>
 </file>
@@ -7179,7 +7198,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$13</c:f>
+              <c:f>SurveyRespond!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7218,7 +7237,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$B$4:$B$13</c:f>
+              <c:f>SurveyRespond!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7294,7 +7313,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7330,7 +7349,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$F$4:$F$12</c:f>
+              <c:f>SurveyRespond!$F$4:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7403,7 +7422,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7439,7 +7458,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$J$4:$J$12</c:f>
+              <c:f>SurveyRespond!$J$4:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7512,7 +7531,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$11</c:f>
+              <c:f>SurveyRespond!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7545,7 +7564,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$N$4:$N$11</c:f>
+              <c:f>SurveyRespond!$N$4:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8028,7 +8047,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$13</c:f>
+              <c:f>SurveyRespond!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8067,7 +8086,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$D$4:$D$13</c:f>
+              <c:f>SurveyRespond!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8143,7 +8162,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -8179,7 +8198,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$H$4:$H$12</c:f>
+              <c:f>SurveyRespond!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -8252,7 +8271,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -8288,7 +8307,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$L$4:$L$12</c:f>
+              <c:f>SurveyRespond!$L$4:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -8361,7 +8380,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$11</c:f>
+              <c:f>SurveyRespond!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8394,7 +8413,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$P$4:$P$11</c:f>
+              <c:f>SurveyRespond!$P$4:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8877,7 +8896,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$13</c:f>
+              <c:f>SurveyRespond!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8916,7 +8935,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$C$4:$C$13</c:f>
+              <c:f>SurveyRespond!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8992,7 +9011,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9028,7 +9047,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$G$4:$G$12</c:f>
+              <c:f>SurveyRespond!$G$4:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9101,7 +9120,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9137,7 +9156,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$K$4:$K$12</c:f>
+              <c:f>SurveyRespond!$K$4:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9210,7 +9229,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$11</c:f>
+              <c:f>SurveyRespond!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9243,7 +9262,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$O$4:$O$11</c:f>
+              <c:f>SurveyRespond!$O$4:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -10440,7 +10459,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$13</c:f>
+              <c:f>SurveyRespond!$A$4:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10479,7 +10498,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$E$4:$E$13</c:f>
+              <c:f>SurveyRespond!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10555,7 +10574,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10591,7 +10610,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$I$4:$I$12</c:f>
+              <c:f>SurveyRespond!$I$4:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10664,7 +10683,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$12</c:f>
+              <c:f>SurveyRespond!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10700,7 +10719,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$M$4:$M$12</c:f>
+              <c:f>SurveyRespond!$M$4:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10773,7 +10792,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$4:$A$11</c:f>
+              <c:f>SurveyRespond!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -10806,7 +10825,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$Q$4:$Q$11</c:f>
+              <c:f>SurveyRespond!$Q$4:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -11292,7 +11311,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$57:$A$65</c:f>
+              <c:f>SurveyRespond!$A$57:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11328,7 +11347,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$B$56:$B$65</c:f>
+              <c:f>SurveyRespond!$B$56:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -11404,7 +11423,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11440,7 +11459,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$F$56:$F$64</c:f>
+              <c:f>SurveyRespond!$F$56:$F$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11513,7 +11532,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11549,7 +11568,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$J$56:$J$64</c:f>
+              <c:f>SurveyRespond!$J$56:$J$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11622,7 +11641,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$63</c:f>
+              <c:f>SurveyRespond!$A$56:$A$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -11655,7 +11674,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$N$56:$N$63</c:f>
+              <c:f>SurveyRespond!$N$56:$N$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -12138,7 +12157,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$65</c:f>
+              <c:f>SurveyRespond!$A$56:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -12177,7 +12196,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$D$56:$D$65</c:f>
+              <c:f>SurveyRespond!$D$56:$D$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -12253,7 +12272,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12289,7 +12308,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$H$56:$H$64</c:f>
+              <c:f>SurveyRespond!$H$56:$H$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12362,7 +12381,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12398,7 +12417,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$L$56:$L$64</c:f>
+              <c:f>SurveyRespond!$L$56:$L$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12471,7 +12490,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$63</c:f>
+              <c:f>SurveyRespond!$A$56:$A$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -12504,7 +12523,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$P$56:$P$63</c:f>
+              <c:f>SurveyRespond!$P$56:$P$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -12982,7 +13001,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$65</c:f>
+              <c:f>SurveyRespond!$A$56:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -13021,7 +13040,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$C$56:$C$65</c:f>
+              <c:f>SurveyRespond!$C$56:$C$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -13097,7 +13116,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -13133,7 +13152,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$G$56:$G$64</c:f>
+              <c:f>SurveyRespond!$G$56:$G$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -13206,7 +13225,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -13242,7 +13261,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$K$56:$K$64</c:f>
+              <c:f>SurveyRespond!$K$56:$K$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -13315,7 +13334,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$63</c:f>
+              <c:f>SurveyRespond!$A$56:$A$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -13348,7 +13367,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$O$56:$O$63</c:f>
+              <c:f>SurveyRespond!$O$56:$O$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -13834,7 +13853,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$65</c:f>
+              <c:f>SurveyRespond!$A$56:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -13873,7 +13892,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$E$56:$E$65</c:f>
+              <c:f>SurveyRespond!$E$56:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -13949,7 +13968,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -13985,7 +14004,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$I$56:$I$64</c:f>
+              <c:f>SurveyRespond!$I$56:$I$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14058,7 +14077,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$64</c:f>
+              <c:f>SurveyRespond!$A$56:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14094,7 +14113,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$M$56:$M$64</c:f>
+              <c:f>SurveyRespond!$M$56:$M$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14167,7 +14186,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$56:$A$63</c:f>
+              <c:f>SurveyRespond!$A$56:$A$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -14200,7 +14219,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$Q$56:$Q$63</c:f>
+              <c:f>SurveyRespond!$Q$56:$Q$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -14693,7 +14712,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$109</c:f>
+              <c:f>SurveyRespond!$A$100:$A$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -14732,7 +14751,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$B$100:$B$109</c:f>
+              <c:f>SurveyRespond!$B$100:$B$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -14808,7 +14827,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14844,7 +14863,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$F$100:$F$108</c:f>
+              <c:f>SurveyRespond!$F$100:$F$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14917,7 +14936,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14953,7 +14972,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$J$100:$J$108</c:f>
+              <c:f>SurveyRespond!$J$100:$J$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15026,7 +15045,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$107</c:f>
+              <c:f>SurveyRespond!$A$100:$A$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -15059,7 +15078,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$N$100:$N$107</c:f>
+              <c:f>SurveyRespond!$N$100:$N$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -15537,7 +15556,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$101:$A$109</c:f>
+              <c:f>SurveyRespond!$A$101:$A$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15573,7 +15592,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$D$100:$D$109</c:f>
+              <c:f>SurveyRespond!$D$100:$D$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -15649,7 +15668,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15685,7 +15704,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$H$100:$H$108</c:f>
+              <c:f>SurveyRespond!$H$100:$H$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15758,7 +15777,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15794,7 +15813,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$L$100:$L$108</c:f>
+              <c:f>SurveyRespond!$L$100:$L$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -15867,7 +15886,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$107</c:f>
+              <c:f>SurveyRespond!$A$100:$A$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -15900,7 +15919,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$P$100:$P$107</c:f>
+              <c:f>SurveyRespond!$P$100:$P$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -16378,7 +16397,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$109</c:f>
+              <c:f>SurveyRespond!$A$100:$A$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -16417,7 +16436,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$C$100:$C$109</c:f>
+              <c:f>SurveyRespond!$C$100:$C$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -16493,7 +16512,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16529,7 +16548,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$G$100:$G$108</c:f>
+              <c:f>SurveyRespond!$G$100:$G$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16602,7 +16621,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16638,7 +16657,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$K$100:$K$108</c:f>
+              <c:f>SurveyRespond!$K$100:$K$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16711,7 +16730,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$107</c:f>
+              <c:f>SurveyRespond!$A$100:$A$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -16744,7 +16763,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$O$100:$O$107</c:f>
+              <c:f>SurveyRespond!$O$100:$O$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -17217,7 +17236,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$109</c:f>
+              <c:f>SurveyRespond!$A$100:$A$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -17256,7 +17275,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$E$100:$E$109</c:f>
+              <c:f>SurveyRespond!$E$100:$E$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -17332,7 +17351,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17368,7 +17387,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$G$100:$G$108</c:f>
+              <c:f>SurveyRespond!$G$100:$G$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17441,7 +17460,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$108</c:f>
+              <c:f>SurveyRespond!$A$100:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17477,7 +17496,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$M$100:$M$108</c:f>
+              <c:f>SurveyRespond!$M$100:$M$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17550,7 +17569,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$A$100:$A$107</c:f>
+              <c:f>SurveyRespond!$A$100:$A$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -17583,7 +17602,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SurveyRespnod!$Q$100:$Q$107</c:f>
+              <c:f>SurveyRespond!$Q$100:$Q$107</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -43715,8 +43734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3168BB-833A-4FB7-A9ED-74D6E2A3DEE5}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="K148" sqref="K148"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45731,4 +45750,232 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63892896-5A85-4918-B0F2-171D3A52426A}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1024</v>
+      </c>
+      <c r="B5">
+        <v>4323</v>
+      </c>
+      <c r="C5">
+        <v>4323</v>
+      </c>
+      <c r="E5">
+        <v>2396</v>
+      </c>
+      <c r="F5">
+        <v>2396</v>
+      </c>
+      <c r="H5">
+        <v>1958</v>
+      </c>
+      <c r="I5">
+        <v>1958</v>
+      </c>
+      <c r="K5">
+        <v>1814</v>
+      </c>
+      <c r="L5">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2048</v>
+      </c>
+      <c r="B6">
+        <v>4433</v>
+      </c>
+      <c r="C6">
+        <v>8866</v>
+      </c>
+      <c r="E6">
+        <v>2387</v>
+      </c>
+      <c r="F6">
+        <v>4774</v>
+      </c>
+      <c r="H6">
+        <v>1986</v>
+      </c>
+      <c r="I6">
+        <v>3971</v>
+      </c>
+      <c r="K6">
+        <v>1660</v>
+      </c>
+      <c r="L6">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4096</v>
+      </c>
+      <c r="B7">
+        <v>4901</v>
+      </c>
+      <c r="C7">
+        <v>16902</v>
+      </c>
+      <c r="E7">
+        <v>2272</v>
+      </c>
+      <c r="F7">
+        <v>9087</v>
+      </c>
+      <c r="H7">
+        <v>1834</v>
+      </c>
+      <c r="I7">
+        <v>7336</v>
+      </c>
+      <c r="K7">
+        <v>1841</v>
+      </c>
+      <c r="L7">
+        <v>7366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8192</v>
+      </c>
+      <c r="B8">
+        <v>4794</v>
+      </c>
+      <c r="C8">
+        <v>38348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1048576</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Incorporate updated bus timings.
</commit_message>
<xml_diff>
--- a/performance/Performance.xlsx
+++ b/performance/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\ron\nnmg\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634AD0F-2222-4422-910E-CF4EE7281D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9FB9FE-3BB9-440D-A35D-27D6794BFB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="1890" windowWidth="28890" windowHeight="12645" activeTab="6" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
+    <workbookView xWindow="-37880" yWindow="-9300" windowWidth="37390" windowHeight="9710" activeTab="6" xr2:uid="{C17589B4-3E3B-472E-9C23-2794327D84AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Pair timings" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="61">
   <si>
     <t>Pair</t>
   </si>
@@ -220,12 +220,18 @@
   <si>
     <t>IPC</t>
   </si>
+  <si>
+    <t xml:space="preserve">Note: Did not believe the n=2 measurement so redid. </t>
+  </si>
+  <si>
+    <t>Wrong size in script, redid by hand</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +246,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -271,6 +283,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18135,37 +18151,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4323</c:v>
+                  <c:v>4352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4433</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4901</c:v>
+                  <c:v>4621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4794</c:v>
+                  <c:v>4640</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5034</c:v>
+                  <c:v>4732</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5154</c:v>
+                  <c:v>4836</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5271</c:v>
+                  <c:v>5183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5673</c:v>
+                  <c:v>5096</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6206</c:v>
+                  <c:v>5266</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6727</c:v>
+                  <c:v>5306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6175</c:v>
+                  <c:v>6313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18256,37 +18272,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2396</c:v>
+                  <c:v>1776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2387</c:v>
+                  <c:v>2356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2272</c:v>
+                  <c:v>2279</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2390</c:v>
+                  <c:v>2411</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2466</c:v>
+                  <c:v>2482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2589</c:v>
+                  <c:v>2604</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2871</c:v>
+                  <c:v>2731</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2766</c:v>
+                  <c:v>2812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3508</c:v>
+                  <c:v>3011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2653</c:v>
+                  <c:v>1735</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1316</c:v>
+                  <c:v>1407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18377,37 +18393,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1958</c:v>
+                  <c:v>1739</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1986</c:v>
+                  <c:v>1884</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1834</c:v>
+                  <c:v>1893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1865</c:v>
+                  <c:v>1877</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1798</c:v>
+                  <c:v>1856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1890</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1656</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1470</c:v>
+                  <c:v>1486</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1774</c:v>
+                  <c:v>1354</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>999</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>593</c:v>
+                  <c:v>611</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18498,37 +18514,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1814</c:v>
+                  <c:v>1794</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1787</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1652</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1660</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1841</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1740</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1647</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1564</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1407</c:v>
+                  <c:v>1387</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1169</c:v>
+                  <c:v>1069</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>874</c:v>
+                  <c:v>707</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>687</c:v>
+                  <c:v>562</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>435</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19915,37 +19931,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4323</c:v>
+                  <c:v>4352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8866</c:v>
+                  <c:v>9199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16902</c:v>
+                  <c:v>18483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38348</c:v>
+                  <c:v>37123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80548</c:v>
+                  <c:v>75705</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>164926</c:v>
+                  <c:v>154770</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>337362</c:v>
+                  <c:v>331704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>726140</c:v>
+                  <c:v>652282</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1600000</c:v>
+                  <c:v>1300000</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>3400000</c:v>
+                  <c:v>2700000</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>6300000</c:v>
+                  <c:v>6400000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20036,37 +20052,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2396</c:v>
+                  <c:v>1776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4774</c:v>
+                  <c:v>4712</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9087</c:v>
+                  <c:v>9116</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19120</c:v>
+                  <c:v>19287</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39451</c:v>
+                  <c:v>39706</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82844</c:v>
+                  <c:v>83313</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>183755</c:v>
+                  <c:v>174776</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>354065</c:v>
+                  <c:v>360011</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>782904</c:v>
+                  <c:v>770825</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>888217</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
                   <c:v>1400000</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1350000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20157,37 +20173,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1814</c:v>
+                  <c:v>1794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3321</c:v>
+                  <c:v>1408</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7366</c:v>
+                  <c:v>6828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13925</c:v>
+                  <c:v>14297</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26348</c:v>
+                  <c:v>26438</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50057</c:v>
+                  <c:v>53132</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90049</c:v>
+                  <c:v>88788</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>145629</c:v>
+                  <c:v>136807</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>223897</c:v>
+                  <c:v>180999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>351612</c:v>
+                  <c:v>287609</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>445643</c:v>
+                  <c:v>466298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20278,37 +20294,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1814</c:v>
+                  <c:v>1794</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3321</c:v>
+                  <c:v>1408</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7366</c:v>
+                  <c:v>6828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13925</c:v>
+                  <c:v>14297</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26348</c:v>
+                  <c:v>26438</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50057</c:v>
+                  <c:v>53132</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90049</c:v>
+                  <c:v>88788</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>145629</c:v>
+                  <c:v>136807</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>223897</c:v>
+                  <c:v>180999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>351612</c:v>
+                  <c:v>287609</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>445643</c:v>
+                  <c:v>466298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20770,10 +20786,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Bus!$A$49:$A$57</c:f>
+              <c:f>Bus!$A$49:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -20800,42 +20816,54 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Bus!$B$49:$B$57</c:f>
+              <c:f>Bus!$B$49:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5206</c:v>
+                  <c:v>4350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4796</c:v>
+                  <c:v>4438</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5054</c:v>
+                  <c:v>4874</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4929</c:v>
+                  <c:v>5014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4769</c:v>
+                  <c:v>4974</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4943</c:v>
+                  <c:v>3791</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5199</c:v>
+                  <c:v>4617</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5550</c:v>
+                  <c:v>5124</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6198</c:v>
+                  <c:v>5883</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6012</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20926,37 +20954,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2611</c:v>
+                  <c:v>1349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2375</c:v>
+                  <c:v>2728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2472</c:v>
+                  <c:v>2474</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2726</c:v>
+                  <c:v>2941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2746</c:v>
+                  <c:v>2549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3086</c:v>
+                  <c:v>2161</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2868</c:v>
+                  <c:v>2320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2956</c:v>
+                  <c:v>2401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3469</c:v>
+                  <c:v>2747</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3076</c:v>
+                  <c:v>2733</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2111</c:v>
+                  <c:v>2281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21047,37 +21075,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1828</c:v>
+                  <c:v>1447</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1918</c:v>
+                  <c:v>1495</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1817</c:v>
+                  <c:v>1506</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1820</c:v>
+                  <c:v>1789</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1874</c:v>
+                  <c:v>1937</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1627</c:v>
+                  <c:v>1681</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2022</c:v>
+                  <c:v>1465</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2202</c:v>
+                  <c:v>1793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2451</c:v>
+                  <c:v>2076</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2517</c:v>
+                  <c:v>1836</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1560</c:v>
+                  <c:v>1544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21121,10 +21149,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Bus!$A$49:$A$58</c:f>
+              <c:f>Bus!$A$49:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -21154,45 +21182,51 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Bus!$K$49:$K$58</c:f>
+              <c:f>Bus!$K$49:$K$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1768</c:v>
+                  <c:v>1376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1734</c:v>
+                  <c:v>1364</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1675</c:v>
+                  <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1623</c:v>
+                  <c:v>1339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1655</c:v>
+                  <c:v>1489</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1587</c:v>
+                  <c:v>1548</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1720</c:v>
+                  <c:v>1465</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1903</c:v>
+                  <c:v>1519</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2104</c:v>
+                  <c:v>1654</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2192</c:v>
+                  <c:v>1510</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1362</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21649,10 +21683,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Bus!$A$49:$A$57</c:f>
+              <c:f>Bus!$A$49:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -21679,42 +21713,54 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Bus!$C$49:$C$57</c:f>
+              <c:f>Bus!$C$49:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5206</c:v>
+                  <c:v>4350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9592</c:v>
+                  <c:v>8877</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20215</c:v>
+                  <c:v>19495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39435</c:v>
+                  <c:v>40116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76304</c:v>
+                  <c:v>79580</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15818</c:v>
+                  <c:v>121310</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>332727</c:v>
+                  <c:v>295477</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>710365</c:v>
+                  <c:v>655918</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1590000</c:v>
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00E+00">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>7100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21805,37 +21851,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2166</c:v>
+                  <c:v>1349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4749</c:v>
+                  <c:v>5455</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9887</c:v>
+                  <c:v>9895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21812</c:v>
+                  <c:v>23526</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43932</c:v>
+                  <c:v>40781</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98741</c:v>
+                  <c:v>69138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>183554</c:v>
+                  <c:v>148481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>378391</c:v>
+                  <c:v>307359</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>888019</c:v>
+                  <c:v>703231</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1570000</c:v>
+                  <c:v>1400000</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>2160000</c:v>
+                  <c:v>2300000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21926,34 +21972,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1828</c:v>
+                  <c:v>1447</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3835</c:v>
+                  <c:v>2990</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7268</c:v>
+                  <c:v>6023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14564</c:v>
+                  <c:v>14313</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29990</c:v>
+                  <c:v>30990</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52053</c:v>
+                  <c:v>53796</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>129404</c:v>
+                  <c:v>93770</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>281808</c:v>
+                  <c:v>229467</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>627384</c:v>
+                  <c:v>531396</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1290000</c:v>
+                  <c:v>940164</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
                   <c:v>1600000</c:v>
@@ -22000,10 +22046,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Bus!$A$49:$A$58</c:f>
+              <c:f>Bus!$A$49:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1024</c:v>
                 </c:pt>
@@ -22033,45 +22079,51 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Bus!$L$49:$L$58</c:f>
+              <c:f>Bus!$L$49:$L$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1768</c:v>
+                  <c:v>1376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3468</c:v>
+                  <c:v>2729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6702</c:v>
+                  <c:v>5839</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12987</c:v>
+                  <c:v>10713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26483</c:v>
+                  <c:v>23819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50786</c:v>
+                  <c:v>19536</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>110112</c:v>
+                  <c:v>93770</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>243582</c:v>
+                  <c:v>194393</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>538551</c:v>
+                  <c:v>423383</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1220000</c:v>
+                  <c:v>773385</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>1400000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22565,37 +22617,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4913</c:v>
+                  <c:v>4739</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4532</c:v>
+                  <c:v>3621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4692</c:v>
+                  <c:v>3632</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4714</c:v>
+                  <c:v>4733</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4402</c:v>
+                  <c:v>4559</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4642</c:v>
+                  <c:v>3749</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4717</c:v>
+                  <c:v>3758</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4694</c:v>
+                  <c:v>4901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4774</c:v>
+                  <c:v>4684</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4460</c:v>
+                  <c:v>3594</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3979</c:v>
+                  <c:v>3394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22686,37 +22738,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3245</c:v>
+                  <c:v>2665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3023</c:v>
+                  <c:v>2103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2740</c:v>
+                  <c:v>2670</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2645</c:v>
+                  <c:v>2208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2615</c:v>
+                  <c:v>2530</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2611</c:v>
+                  <c:v>2118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2512</c:v>
+                  <c:v>1937</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2335</c:v>
+                  <c:v>2409</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2256</c:v>
+                  <c:v>2169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2153</c:v>
+                  <c:v>1736</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1856</c:v>
+                  <c:v>1797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22807,37 +22859,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2200</c:v>
+                  <c:v>2158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2279</c:v>
+                  <c:v>1572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2080</c:v>
+                  <c:v>2066</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2063</c:v>
+                  <c:v>2032</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2037</c:v>
+                  <c:v>1617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2076</c:v>
+                  <c:v>1519</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1934</c:v>
+                  <c:v>1431</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1750</c:v>
+                  <c:v>1666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1579</c:v>
+                  <c:v>1507</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1508</c:v>
+                  <c:v>1184</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1302</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22928,37 +22980,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1720</c:v>
+                  <c:v>1403</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1935</c:v>
+                  <c:v>1433</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1765</c:v>
+                  <c:v>1780</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1908</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1715</c:v>
+                  <c:v>1385</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1623</c:v>
+                  <c:v>1292</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1596</c:v>
+                  <c:v>1493</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1421</c:v>
+                  <c:v>1164</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1298</c:v>
+                  <c:v>1058</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1256</c:v>
+                  <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>868</c:v>
+                  <c:v>841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23452,37 +23504,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4913</c:v>
+                  <c:v>4739</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9064</c:v>
+                  <c:v>7242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18770</c:v>
+                  <c:v>14527</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37713</c:v>
+                  <c:v>37861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70427</c:v>
+                  <c:v>72950</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>148548</c:v>
+                  <c:v>119958</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>301908</c:v>
+                  <c:v>240480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>102151</c:v>
+                  <c:v>627344</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1220000</c:v>
+                  <c:v>1200000</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>2280000</c:v>
+                  <c:v>1800000</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>4070000</c:v>
+                  <c:v>3500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23573,37 +23625,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>3245</c:v>
+                  <c:v>2665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6045</c:v>
+                  <c:v>4206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10959</c:v>
+                  <c:v>10680</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21158</c:v>
+                  <c:v>17666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41840</c:v>
+                  <c:v>40483</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83548</c:v>
+                  <c:v>67793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160793</c:v>
+                  <c:v>123965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>298885</c:v>
+                  <c:v>308345</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>577685</c:v>
+                  <c:v>555277</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>1100000</c:v>
+                  <c:v>888900</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1930000</c:v>
+                  <c:v>1800000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23694,37 +23746,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2200</c:v>
+                  <c:v>2158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4559</c:v>
+                  <c:v>3143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8320</c:v>
+                  <c:v>8266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16503</c:v>
+                  <c:v>16256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32591</c:v>
+                  <c:v>25867</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66419</c:v>
+                  <c:v>48618</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123744</c:v>
+                  <c:v>91579</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>223944</c:v>
+                  <c:v>213220</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>404344</c:v>
+                  <c:v>385870</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>772007</c:v>
+                  <c:v>606553</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>1330000</c:v>
+                  <c:v>1300000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23815,37 +23867,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1720</c:v>
+                  <c:v>1403</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3870</c:v>
+                  <c:v>2867</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7059</c:v>
+                  <c:v>7119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15261</c:v>
+                  <c:v>14554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27454</c:v>
+                  <c:v>22157</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51935</c:v>
+                  <c:v>41331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102151</c:v>
+                  <c:v>95542</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>181918</c:v>
+                  <c:v>149035</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>332233</c:v>
+                  <c:v>270981</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>642874</c:v>
+                  <c:v>399130</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>889446</c:v>
+                  <c:v>861486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -54635,18 +54687,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63892896-5A85-4918-B0F2-171D3A52426A}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="V132" sqref="V132"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="M103" sqref="M103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -54667,12 +54720,12 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -54689,7 +54742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -54718,323 +54771,336 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1024</v>
       </c>
       <c r="B5">
-        <v>4323</v>
+        <v>4352</v>
       </c>
       <c r="C5">
-        <v>4323</v>
+        <v>4352</v>
       </c>
       <c r="E5">
-        <v>2396</v>
+        <v>1776</v>
       </c>
       <c r="F5">
-        <v>2396</v>
+        <v>1776</v>
       </c>
       <c r="H5">
-        <v>1958</v>
+        <v>1739</v>
       </c>
       <c r="I5">
-        <v>1958</v>
+        <v>1739</v>
       </c>
       <c r="K5">
-        <v>1814</v>
+        <v>1794</v>
       </c>
       <c r="L5">
-        <v>1814</v>
+        <v>1794</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2048</v>
       </c>
       <c r="B6">
-        <v>4433</v>
+        <v>4600</v>
       </c>
       <c r="C6">
-        <v>8866</v>
+        <v>9199</v>
       </c>
       <c r="E6">
-        <v>2387</v>
+        <v>2356</v>
       </c>
       <c r="F6">
-        <v>4774</v>
+        <v>4712</v>
       </c>
       <c r="H6">
-        <v>1986</v>
+        <v>1884</v>
       </c>
       <c r="I6">
-        <v>3971</v>
+        <v>3768</v>
       </c>
       <c r="K6">
-        <v>1660</v>
+        <v>1704</v>
       </c>
       <c r="L6">
-        <v>3321</v>
+        <v>1408</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4096</v>
       </c>
       <c r="B7">
-        <v>4901</v>
+        <v>4621</v>
       </c>
       <c r="C7">
-        <v>16902</v>
+        <v>18483</v>
       </c>
       <c r="E7">
-        <v>2272</v>
+        <v>2279</v>
       </c>
       <c r="F7">
-        <v>9087</v>
+        <v>9116</v>
       </c>
       <c r="H7">
-        <v>1834</v>
+        <v>1893</v>
       </c>
       <c r="I7">
-        <v>7336</v>
+        <v>7543</v>
       </c>
       <c r="K7">
-        <v>1841</v>
+        <v>1707</v>
       </c>
       <c r="L7">
-        <v>7366</v>
+        <v>6828</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8192</v>
       </c>
       <c r="B8">
-        <v>4794</v>
+        <v>4640</v>
       </c>
       <c r="C8">
-        <v>38348</v>
+        <v>37123</v>
       </c>
       <c r="E8">
-        <v>2390</v>
+        <v>2411</v>
       </c>
       <c r="F8">
-        <v>19120</v>
+        <v>19287</v>
       </c>
       <c r="H8">
-        <v>1865</v>
+        <v>1877</v>
       </c>
       <c r="I8">
-        <v>14920</v>
+        <v>15017</v>
       </c>
       <c r="K8">
-        <v>1740</v>
+        <v>1787</v>
       </c>
       <c r="L8">
-        <v>13925</v>
+        <v>14297</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16384</v>
       </c>
       <c r="B9">
-        <v>5034</v>
+        <v>4732</v>
       </c>
       <c r="C9">
-        <v>80548</v>
+        <v>75705</v>
       </c>
       <c r="E9">
-        <v>2466</v>
+        <v>2482</v>
       </c>
       <c r="F9">
-        <v>39451</v>
+        <v>39706</v>
       </c>
       <c r="H9">
-        <v>1798</v>
+        <v>1856</v>
       </c>
       <c r="I9">
-        <v>28768</v>
+        <v>29692</v>
       </c>
       <c r="K9">
-        <v>1647</v>
+        <v>1652</v>
       </c>
       <c r="L9">
-        <v>26348</v>
+        <v>26438</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>32768</v>
       </c>
       <c r="B10">
-        <v>5154</v>
+        <v>4836</v>
       </c>
       <c r="C10">
-        <v>164926</v>
+        <v>154770</v>
       </c>
       <c r="E10">
-        <v>2589</v>
+        <v>2604</v>
       </c>
       <c r="F10">
-        <v>82844</v>
+        <v>83313</v>
       </c>
       <c r="H10">
-        <v>1890</v>
+        <v>2011</v>
       </c>
       <c r="I10">
-        <v>60480</v>
+        <v>64360</v>
       </c>
       <c r="K10">
-        <v>1564</v>
+        <v>1660</v>
       </c>
       <c r="L10">
-        <v>50057</v>
+        <v>53132</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>65536</v>
       </c>
       <c r="B11">
-        <v>5271</v>
+        <v>5183</v>
       </c>
       <c r="C11">
-        <v>337362</v>
+        <v>331704</v>
       </c>
       <c r="E11">
-        <v>2871</v>
+        <v>2731</v>
       </c>
       <c r="F11">
-        <v>183755</v>
+        <v>174776</v>
       </c>
       <c r="H11">
-        <v>1656</v>
+        <v>1650</v>
       </c>
       <c r="I11">
-        <v>105953</v>
+        <v>105592</v>
       </c>
       <c r="K11">
-        <v>1407</v>
+        <v>1387</v>
       </c>
       <c r="L11">
-        <v>90049</v>
+        <v>88788</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>131072</v>
       </c>
       <c r="B12">
-        <v>5673</v>
+        <v>5096</v>
       </c>
       <c r="C12">
-        <v>726140</v>
+        <v>652282</v>
       </c>
       <c r="E12">
-        <v>2766</v>
+        <v>2812</v>
       </c>
       <c r="F12">
-        <v>354065</v>
+        <v>360011</v>
       </c>
       <c r="H12">
-        <v>1470</v>
+        <v>1486</v>
       </c>
       <c r="I12">
-        <v>188193</v>
+        <v>190168</v>
       </c>
       <c r="K12">
-        <v>1169</v>
+        <v>1069</v>
       </c>
       <c r="L12">
-        <v>145629</v>
-      </c>
+        <v>136807</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>262144</v>
       </c>
       <c r="B13">
-        <v>6206</v>
+        <v>5266</v>
       </c>
       <c r="C13" s="2">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="E13">
-        <v>3508</v>
+        <v>3011</v>
       </c>
       <c r="F13">
-        <v>782904</v>
+        <v>770825</v>
       </c>
       <c r="H13">
-        <v>1774</v>
+        <v>1354</v>
       </c>
       <c r="I13">
-        <v>454279</v>
+        <v>346752</v>
       </c>
       <c r="K13">
-        <v>874</v>
-      </c>
-      <c r="L13">
-        <v>223897</v>
+        <v>707</v>
+      </c>
+      <c r="L13" s="7">
+        <v>180999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>524288</v>
       </c>
       <c r="B14">
-        <v>6727</v>
+        <v>5306</v>
       </c>
       <c r="C14" s="2">
-        <v>3400000</v>
+        <v>2700000</v>
       </c>
       <c r="E14">
-        <v>2653</v>
+        <v>1735</v>
       </c>
       <c r="F14" s="2">
-        <v>1400000</v>
+        <v>888217</v>
       </c>
       <c r="H14">
-        <v>999</v>
+        <v>850</v>
       </c>
       <c r="I14">
-        <v>511440</v>
+        <v>435368</v>
       </c>
       <c r="K14">
-        <v>687</v>
+        <v>562</v>
       </c>
       <c r="L14">
-        <v>351612</v>
-      </c>
+        <v>287609</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1048576</v>
       </c>
       <c r="B15">
-        <v>6175</v>
+        <v>6313</v>
       </c>
       <c r="C15" s="2">
-        <v>6300000</v>
+        <v>6400000</v>
       </c>
       <c r="E15">
-        <v>1316</v>
+        <v>1407</v>
       </c>
       <c r="F15" s="2">
-        <v>1350000</v>
+        <v>1400000</v>
       </c>
       <c r="H15">
-        <v>593</v>
+        <v>611</v>
       </c>
       <c r="I15">
-        <v>606988</v>
+        <v>626589</v>
       </c>
       <c r="K15">
-        <v>435</v>
+        <v>455</v>
       </c>
       <c r="L15">
-        <v>445643</v>
+        <v>466298</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -55071,335 +55137,352 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1024</v>
       </c>
       <c r="B49">
-        <v>5206</v>
+        <v>4350</v>
       </c>
       <c r="C49">
-        <v>5206</v>
+        <v>4350</v>
       </c>
       <c r="E49">
-        <v>2611</v>
+        <v>1349</v>
       </c>
       <c r="F49">
-        <v>2166</v>
+        <v>1349</v>
       </c>
       <c r="H49">
-        <v>1828</v>
+        <v>1447</v>
       </c>
       <c r="I49">
-        <v>1828</v>
+        <v>1447</v>
       </c>
       <c r="K49">
-        <v>1768</v>
+        <v>1376</v>
       </c>
       <c r="L49">
-        <v>1768</v>
+        <v>1376</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2048</v>
       </c>
       <c r="B50">
-        <v>4796</v>
+        <v>4438</v>
       </c>
       <c r="C50">
-        <v>9592</v>
+        <v>8877</v>
       </c>
       <c r="E50">
-        <v>2375</v>
+        <v>2728</v>
       </c>
       <c r="F50">
-        <v>4749</v>
+        <v>5455</v>
       </c>
       <c r="H50">
-        <v>1918</v>
+        <v>1495</v>
       </c>
       <c r="I50">
-        <v>3835</v>
+        <v>2990</v>
       </c>
       <c r="K50">
-        <v>1734</v>
+        <v>1364</v>
       </c>
       <c r="L50">
-        <v>3468</v>
+        <v>2729</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4096</v>
       </c>
       <c r="B51">
-        <v>5054</v>
+        <v>4874</v>
       </c>
       <c r="C51">
-        <v>20215</v>
+        <v>19495</v>
       </c>
       <c r="E51">
-        <v>2472</v>
+        <v>2474</v>
       </c>
       <c r="F51">
-        <v>9887</v>
+        <v>9895</v>
       </c>
       <c r="H51">
-        <v>1817</v>
+        <v>1506</v>
       </c>
       <c r="I51">
-        <v>7268</v>
+        <v>6023</v>
       </c>
       <c r="K51">
-        <v>1675</v>
+        <v>1460</v>
       </c>
       <c r="L51">
-        <v>6702</v>
+        <v>5839</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>8192</v>
       </c>
       <c r="B52">
-        <v>4929</v>
+        <v>5014</v>
       </c>
       <c r="C52">
-        <v>39435</v>
+        <v>40116</v>
       </c>
       <c r="E52">
-        <v>2726</v>
+        <v>2941</v>
       </c>
       <c r="F52">
-        <v>21812</v>
+        <v>23526</v>
       </c>
       <c r="H52">
-        <v>1820</v>
+        <v>1789</v>
       </c>
       <c r="I52">
-        <v>14564</v>
+        <v>14313</v>
       </c>
       <c r="K52">
-        <v>1623</v>
+        <v>1339</v>
       </c>
       <c r="L52">
-        <v>12987</v>
+        <v>10713</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16384</v>
       </c>
       <c r="B53">
-        <v>4769</v>
+        <v>4974</v>
       </c>
       <c r="C53">
-        <v>76304</v>
+        <v>79580</v>
       </c>
       <c r="E53">
-        <v>2746</v>
+        <v>2549</v>
       </c>
       <c r="F53">
-        <v>43932</v>
+        <v>40781</v>
       </c>
       <c r="H53">
-        <v>1874</v>
+        <v>1937</v>
       </c>
       <c r="I53">
-        <v>29990</v>
+        <v>30990</v>
       </c>
       <c r="K53">
-        <v>1655</v>
+        <v>1489</v>
       </c>
       <c r="L53">
-        <v>26483</v>
+        <v>23819</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>32768</v>
       </c>
       <c r="B54">
-        <v>4943</v>
+        <v>3791</v>
       </c>
       <c r="C54">
-        <v>15818</v>
+        <v>121310</v>
       </c>
       <c r="E54">
-        <v>3086</v>
+        <v>2161</v>
       </c>
       <c r="F54">
-        <v>98741</v>
+        <v>69138</v>
       </c>
       <c r="H54">
-        <v>1627</v>
+        <v>1681</v>
       </c>
       <c r="I54">
-        <v>52053</v>
+        <v>53796</v>
       </c>
       <c r="K54">
-        <v>1587</v>
+        <v>1548</v>
       </c>
       <c r="L54">
-        <v>50786</v>
+        <v>19536</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>65536</v>
       </c>
       <c r="B55">
-        <v>5199</v>
+        <v>4617</v>
       </c>
       <c r="C55">
-        <v>332727</v>
+        <v>295477</v>
       </c>
       <c r="E55">
-        <v>2868</v>
+        <v>2320</v>
       </c>
       <c r="F55">
-        <v>183554</v>
+        <v>148481</v>
       </c>
       <c r="H55">
-        <v>2022</v>
+        <v>1465</v>
       </c>
       <c r="I55">
-        <v>129404</v>
+        <v>93770</v>
       </c>
       <c r="K55">
-        <v>1720</v>
+        <v>1465</v>
       </c>
       <c r="L55">
-        <v>110112</v>
+        <v>93770</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>131072</v>
       </c>
       <c r="B56">
-        <v>5550</v>
+        <v>5124</v>
       </c>
       <c r="C56">
-        <v>710365</v>
+        <v>655918</v>
       </c>
       <c r="E56">
-        <v>2956</v>
+        <v>2401</v>
       </c>
       <c r="F56">
-        <v>378391</v>
+        <v>307359</v>
       </c>
       <c r="H56">
-        <v>2202</v>
+        <v>1793</v>
       </c>
       <c r="I56">
-        <v>281808</v>
+        <v>229467</v>
       </c>
       <c r="K56">
-        <v>1903</v>
+        <v>1519</v>
       </c>
       <c r="L56">
-        <v>243582</v>
+        <v>194393</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>262144</v>
       </c>
       <c r="B57">
-        <v>6198</v>
+        <v>5883</v>
       </c>
       <c r="C57" s="2">
-        <v>1590000</v>
+        <v>1500000</v>
       </c>
       <c r="E57">
-        <v>3469</v>
+        <v>2747</v>
       </c>
       <c r="F57">
-        <v>888019</v>
+        <v>703231</v>
       </c>
       <c r="H57">
-        <v>2451</v>
+        <v>2076</v>
       </c>
       <c r="I57">
-        <v>627384</v>
+        <v>531396</v>
       </c>
       <c r="K57">
-        <v>2104</v>
+        <v>1654</v>
       </c>
       <c r="L57">
-        <v>538551</v>
+        <v>423383</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>524288</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="B58">
+        <v>6012</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3000000</v>
+      </c>
       <c r="E58">
-        <v>3076</v>
+        <v>2733</v>
       </c>
       <c r="F58" s="2">
-        <v>1570000</v>
+        <v>1400000</v>
       </c>
       <c r="H58">
-        <v>2517</v>
+        <v>1836</v>
       </c>
       <c r="I58" s="2">
-        <v>1290000</v>
+        <v>940164</v>
       </c>
       <c r="K58">
-        <v>2192</v>
+        <v>1510</v>
       </c>
       <c r="L58" s="2">
-        <v>1220000</v>
+        <v>773385</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1048576</v>
       </c>
       <c r="B59">
-        <v>6840</v>
+        <v>6955</v>
       </c>
       <c r="C59" s="2">
-        <v>7000000</v>
+        <v>7100000</v>
       </c>
       <c r="E59">
-        <v>2111</v>
+        <v>2281</v>
       </c>
       <c r="F59" s="2">
-        <v>2160000</v>
+        <v>2300000</v>
       </c>
       <c r="H59">
-        <v>1560</v>
+        <v>1544</v>
       </c>
       <c r="I59" s="2">
         <v>1600000</v>
       </c>
+      <c r="K59">
+        <v>1362</v>
+      </c>
+      <c r="L59" s="2">
+        <v>1400000</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" s="2"/>
       <c r="F60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C61" s="2"/>
       <c r="F61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
       <c r="F62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C63" s="2"/>
       <c r="F63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C64" s="2"/>
       <c r="F64" s="2"/>
       <c r="I64" s="2"/>
@@ -55493,28 +55576,28 @@
         <v>1024</v>
       </c>
       <c r="B93">
-        <v>4913</v>
+        <v>4739</v>
       </c>
       <c r="C93">
-        <v>4913</v>
+        <v>4739</v>
       </c>
       <c r="E93">
-        <v>3245</v>
+        <v>2665</v>
       </c>
       <c r="F93">
-        <v>3245</v>
+        <v>2665</v>
       </c>
       <c r="H93">
-        <v>2200</v>
+        <v>2158</v>
       </c>
       <c r="I93">
-        <v>2200</v>
+        <v>2158</v>
       </c>
       <c r="K93">
-        <v>1720</v>
+        <v>1403</v>
       </c>
       <c r="L93">
-        <v>1720</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -55522,28 +55605,28 @@
         <v>2048</v>
       </c>
       <c r="B94">
-        <v>4532</v>
+        <v>3621</v>
       </c>
       <c r="C94">
-        <v>9064</v>
+        <v>7242</v>
       </c>
       <c r="E94">
-        <v>3023</v>
+        <v>2103</v>
       </c>
       <c r="F94">
-        <v>6045</v>
+        <v>4206</v>
       </c>
       <c r="H94">
-        <v>2279</v>
+        <v>1572</v>
       </c>
       <c r="I94">
-        <v>4559</v>
+        <v>3143</v>
       </c>
       <c r="K94">
-        <v>1935</v>
+        <v>1433</v>
       </c>
       <c r="L94">
-        <v>3870</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -55551,28 +55634,28 @@
         <v>4096</v>
       </c>
       <c r="B95">
-        <v>4692</v>
+        <v>3632</v>
       </c>
       <c r="C95">
-        <v>18770</v>
+        <v>14527</v>
       </c>
       <c r="E95">
-        <v>2740</v>
+        <v>2670</v>
       </c>
       <c r="F95">
-        <v>10959</v>
+        <v>10680</v>
       </c>
       <c r="H95">
-        <v>2080</v>
+        <v>2066</v>
       </c>
       <c r="I95">
-        <v>8320</v>
+        <v>8266</v>
       </c>
       <c r="K95">
-        <v>1765</v>
+        <v>1780</v>
       </c>
       <c r="L95">
-        <v>7059</v>
+        <v>7119</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -55580,238 +55663,248 @@
         <v>8192</v>
       </c>
       <c r="B96">
-        <v>4714</v>
+        <v>4733</v>
       </c>
       <c r="C96">
-        <v>37713</v>
+        <v>37861</v>
       </c>
       <c r="E96">
-        <v>2645</v>
+        <v>2208</v>
       </c>
       <c r="F96">
-        <v>21158</v>
+        <v>17666</v>
       </c>
       <c r="H96">
-        <v>2063</v>
+        <v>2032</v>
       </c>
       <c r="I96">
-        <v>16503</v>
+        <v>16256</v>
       </c>
       <c r="K96">
-        <v>1908</v>
+        <v>1819</v>
       </c>
       <c r="L96">
-        <v>15261</v>
+        <v>14554</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>16384</v>
       </c>
       <c r="B97">
-        <v>4402</v>
+        <v>4559</v>
       </c>
       <c r="C97">
-        <v>70427</v>
+        <v>72950</v>
       </c>
       <c r="E97">
-        <v>2615</v>
+        <v>2530</v>
       </c>
       <c r="F97">
-        <v>41840</v>
+        <v>40483</v>
       </c>
       <c r="H97">
-        <v>2037</v>
+        <v>1617</v>
       </c>
       <c r="I97">
-        <v>32591</v>
+        <v>25867</v>
       </c>
       <c r="K97">
-        <v>1715</v>
+        <v>1385</v>
       </c>
       <c r="L97">
-        <v>27454</v>
+        <v>22157</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>32768</v>
       </c>
       <c r="B98">
-        <v>4642</v>
+        <v>3749</v>
       </c>
       <c r="C98">
-        <v>148548</v>
+        <v>119958</v>
       </c>
       <c r="E98">
-        <v>2611</v>
+        <v>2118</v>
       </c>
       <c r="F98">
-        <v>83548</v>
+        <v>67793</v>
       </c>
       <c r="H98">
-        <v>2076</v>
+        <v>1519</v>
       </c>
       <c r="I98">
-        <v>66419</v>
+        <v>48618</v>
       </c>
       <c r="K98">
-        <v>1623</v>
+        <v>1292</v>
       </c>
       <c r="L98">
-        <v>51935</v>
+        <v>41331</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>65536</v>
       </c>
       <c r="B99">
-        <v>4717</v>
+        <v>3758</v>
       </c>
       <c r="C99">
-        <v>301908</v>
+        <v>240480</v>
       </c>
       <c r="E99">
-        <v>2512</v>
+        <v>1937</v>
       </c>
       <c r="F99">
-        <v>160793</v>
+        <v>123965</v>
       </c>
       <c r="H99">
-        <v>1934</v>
+        <v>1431</v>
       </c>
       <c r="I99">
-        <v>123744</v>
+        <v>91579</v>
       </c>
       <c r="K99">
-        <v>1596</v>
+        <v>1493</v>
       </c>
       <c r="L99">
-        <v>102151</v>
+        <v>95542</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>131072</v>
       </c>
       <c r="B100">
-        <v>4694</v>
+        <v>4901</v>
       </c>
       <c r="C100">
-        <v>102151</v>
+        <v>627344</v>
       </c>
       <c r="E100">
-        <v>2335</v>
+        <v>2409</v>
       </c>
       <c r="F100">
-        <v>298885</v>
+        <v>308345</v>
       </c>
       <c r="H100">
-        <v>1750</v>
+        <v>1666</v>
       </c>
       <c r="I100">
-        <v>223944</v>
+        <v>213220</v>
       </c>
       <c r="K100">
-        <v>1421</v>
+        <v>1164</v>
       </c>
       <c r="L100">
-        <v>181918</v>
+        <v>149035</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>262144</v>
       </c>
       <c r="B101">
-        <v>4774</v>
+        <v>4684</v>
       </c>
       <c r="C101" s="2">
-        <v>1220000</v>
+        <v>1200000</v>
       </c>
       <c r="E101">
-        <v>2256</v>
+        <v>2169</v>
       </c>
       <c r="F101">
-        <v>577685</v>
+        <v>555277</v>
       </c>
       <c r="H101">
-        <v>1579</v>
+        <v>1507</v>
       </c>
       <c r="I101">
-        <v>404344</v>
+        <v>385870</v>
       </c>
       <c r="K101">
-        <v>1298</v>
+        <v>1058</v>
       </c>
       <c r="L101">
-        <v>332233</v>
+        <v>270981</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>524288</v>
       </c>
       <c r="B102">
-        <v>4460</v>
+        <v>3594</v>
       </c>
       <c r="C102" s="2">
-        <v>2280000</v>
+        <v>1800000</v>
       </c>
       <c r="E102">
-        <v>2153</v>
+        <v>1736</v>
       </c>
       <c r="F102" s="2">
-        <v>1100000</v>
+        <v>888900</v>
       </c>
       <c r="H102">
-        <v>1508</v>
+        <v>1184</v>
       </c>
       <c r="I102">
-        <v>772007</v>
+        <v>606553</v>
       </c>
       <c r="K102">
-        <v>1256</v>
+        <v>780</v>
       </c>
       <c r="L102">
-        <v>642874</v>
-      </c>
+        <v>399130</v>
+      </c>
+      <c r="M102" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="6"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1048576</v>
       </c>
       <c r="B103">
-        <v>3979</v>
+        <v>3394</v>
       </c>
       <c r="C103" s="2">
-        <v>4070000</v>
+        <v>3500000</v>
       </c>
       <c r="E103">
-        <v>1856</v>
+        <v>1797</v>
       </c>
       <c r="F103" s="2">
-        <v>1930000</v>
+        <v>1800000</v>
       </c>
       <c r="H103">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="I103" s="2">
-        <v>1330000</v>
+        <v>1300000</v>
       </c>
       <c r="K103">
-        <v>868</v>
+        <v>841</v>
       </c>
       <c r="L103">
-        <v>889446</v>
+        <v>861486</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="M59:P59"/>
+    <mergeCell ref="M102:P102"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>